<commit_message>
New ion radial integrals [some] and SOCs
</commit_message>
<xml_diff>
--- a/Documentation/Ion data.xlsx
+++ b/Documentation/Ion data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shannon\Documents\0Schoolwork\PyCrystalField-mod\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEFABFC-3C7E-4DB5-8A68-F84C8159B1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EAB19D-8C6A-4A50-B0AB-63A16E267815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{EFD51521-650C-4408-8F21-64BF005F46EA}"/>
+    <workbookView xWindow="11730" yWindow="15" windowWidth="11880" windowHeight="12765" xr2:uid="{EFD51521-650C-4408-8F21-64BF005F46EA}"/>
   </bookViews>
   <sheets>
     <sheet name="TM" sheetId="1" r:id="rId1"/>
@@ -3205,7 +3205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3215,6 +3215,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3246,7 +3258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3254,6 +3266,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3591,8 +3608,8 @@
   <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I114" sqref="I114"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81:E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3784,6 +3801,12 @@
       <c r="C8">
         <v>248</v>
       </c>
+      <c r="D8">
+        <v>0.39</v>
+      </c>
+      <c r="E8">
+        <v>0.29499999999999998</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>30</v>
       </c>
@@ -3863,43 +3886,57 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>329</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="D12" s="7">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="7">
         <v>3</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <v>383</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="D13" s="7">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="7">
         <v>2</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="7" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3998,43 +4035,57 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="7">
         <v>479</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="D18" s="7">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="7">
         <v>3</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="7">
         <v>542</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="D19" s="7">
+        <v>0.245</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.112</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="7">
         <v>2</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="7" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4159,26 +4210,26 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="5">
         <v>787</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>3</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="5" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4328,23 +4379,30 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>39</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="7">
         <v>290</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="D33" s="7">
+        <v>1.577</v>
+      </c>
+      <c r="E33" s="7">
+        <v>4.4080000000000004</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="7">
         <v>2</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="7" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4365,618 +4423,737 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="35" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
         <v>40</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>347</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="F35" s="6"/>
+      <c r="G35" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="5">
         <v>3</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="5" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="36" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>40</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="7">
         <v>428</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="D36" s="7">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="E36" s="7">
+        <v>3.09</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="7">
         <v>3</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>40</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="7">
         <v>500</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="D37" s="7">
+        <v>2.645</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2.0129999999999999</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="7">
         <v>2</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>40</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="F38" s="8"/>
+      <c r="G38" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="7">
         <v>0</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="7" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>41</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="7">
         <v>677</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="7">
         <v>0.96</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="7">
         <v>1.573</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="F39" s="8"/>
+      <c r="G39" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="7">
         <v>3</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>41</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="F40" s="8"/>
+      <c r="G40" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="7">
         <v>0</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>42</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="7">
         <v>714</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="D41" s="7">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="7">
         <v>2</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>42</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="7">
         <v>836</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="D42" s="7">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="7">
         <v>3</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="7">
         <v>972</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="D43" s="7">
+        <v>0.747</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="7">
         <v>3</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="7">
         <v>1031</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="D44" s="7">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="7">
         <v>2</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="7" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
         <v>42</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="F45" s="8"/>
+      <c r="G45" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="7">
         <v>0</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>43</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="7">
         <v>1150</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="7">
         <v>0.67400000000000004</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="7">
         <v>0.752</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="F46" s="8"/>
+      <c r="G46" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="7">
         <v>3</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>43</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="F47" s="8"/>
+      <c r="G47" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="7">
         <v>0</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
         <v>44</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="7">
         <v>-942</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="D48" s="7">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1.052</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="7">
         <v>2</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="7" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
         <v>44</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="7">
         <v>1177</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="7">
         <v>0.67400000000000004</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="7">
         <v>0.79</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="F49" s="8"/>
+      <c r="G49" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="7">
         <v>0</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
         <v>44</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="7">
         <v>1350</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="D50" s="7">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="7">
         <v>2</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>44</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="7">
         <v>1700</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="D51" s="7">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="7">
         <v>3</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="7" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="52" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>44</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="F52" s="8"/>
+      <c r="G52" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="7">
         <v>0</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="7" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="53" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
         <v>45</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="7">
         <v>-1194</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="D53" s="7">
+        <v>0.68</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0.85</v>
+      </c>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="7">
         <v>3</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
         <v>45</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="7">
         <v>-1360</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="7">
         <v>0.61</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="7">
         <v>0.64900000000000002</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="F54" s="8"/>
+      <c r="G54" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="7">
         <v>2</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="55" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
         <v>45</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="7">
         <v>1350</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="D55" s="7">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="7">
         <v>0</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="56" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
         <v>46</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="7">
         <v>-1293</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="7">
         <v>0.61699999999999999</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="7">
         <v>0.70499999999999996</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="F56" s="8"/>
+      <c r="G56" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="7">
         <v>3</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="57" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>46</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="7">
         <v>-1211</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="7">
         <v>0.55500000000000005</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="7">
         <v>0.54</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="F57" s="8"/>
+      <c r="G57" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="7">
         <v>3</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="58" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>46</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="7">
         <v>-1830</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="D58" s="7">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="7">
         <v>2</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" s="7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="59" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
         <v>47</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="F59" s="8"/>
+      <c r="G59" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="7">
         <v>0</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="60" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
         <v>47</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="7">
         <v>-1843</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="D60" s="7">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="7">
         <v>2</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="7" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="61" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
         <v>47</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="7">
         <v>-1930</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="D61" s="7">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="7">
         <v>3</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="62" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
         <v>48</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="F62" s="8"/>
+      <c r="G62" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="7">
         <v>0</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="63" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
         <v>48</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="F63" s="8"/>
+      <c r="G63" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="7">
         <v>0</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="7" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="64" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
         <v>48</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="7">
         <v>-2325</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="D64" s="7">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="7">
         <v>2</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64" s="7" t="s">
         <v>218</v>
       </c>
     </row>
@@ -5082,43 +5259,57 @@
         <v>217</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row r="71" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
         <v>72</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="7">
         <v>1370</v>
       </c>
-      <c r="G71" s="1" t="s">
+      <c r="D71" s="7">
+        <v>0.159</v>
+      </c>
+      <c r="E71" s="7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F71" s="8"/>
+      <c r="G71" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="7">
         <v>3</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I71" s="7" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A72">
+    <row r="72" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
         <v>72</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="7">
         <v>1877</v>
       </c>
-      <c r="G72" s="1" t="s">
+      <c r="D72" s="7">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E72" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="F72" s="8"/>
+      <c r="G72" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="7">
         <v>2</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" s="7" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5156,63 +5347,66 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="75" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
         <v>73</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="5">
         <v>2000</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="F75" s="6"/>
+      <c r="G75" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="5">
         <v>3</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="76" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
         <v>73</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="5">
         <v>2254</v>
       </c>
-      <c r="G76" s="1" t="s">
+      <c r="F76" s="6"/>
+      <c r="G76" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="5">
         <v>3</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" s="5" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="77" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
         <v>73</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="5">
         <v>2643</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="F77" s="6"/>
+      <c r="G77" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="5">
         <v>2</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" s="5" t="s">
         <v>229</v>
       </c>
     </row>
@@ -5233,43 +5427,45 @@
         <v>230</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row r="79" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
         <v>74</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="5">
         <v>2500</v>
       </c>
-      <c r="G79" s="1" t="s">
+      <c r="F79" s="6"/>
+      <c r="G79" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="5">
         <v>2</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I79" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row r="80" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
         <v>74</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="5">
         <v>2686</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="F80" s="6"/>
+      <c r="G80" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="5">
         <v>3</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" s="5" t="s">
         <v>232</v>
       </c>
     </row>
@@ -5283,11 +5479,11 @@
       <c r="C81">
         <v>3108</v>
       </c>
-      <c r="D81">
-        <v>0.88039999999999996</v>
-      </c>
-      <c r="E81">
-        <v>1.2311000000000001</v>
+      <c r="D81" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="E81" s="9">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>33</v>
@@ -5312,11 +5508,11 @@
       <c r="C82">
         <v>3483</v>
       </c>
-      <c r="D82">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="E82">
-        <v>0.99299999999999999</v>
+      <c r="D82" s="9">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E82" s="9">
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>33</v>
@@ -5342,10 +5538,10 @@
         <v>5070</v>
       </c>
       <c r="D83">
-        <v>0.1205</v>
+        <v>0.121</v>
       </c>
       <c r="E83">
-        <v>3.1199999999999999E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>33</v>
@@ -5377,63 +5573,66 @@
         <v>234</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="85" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
         <v>75</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="5">
         <v>5800</v>
       </c>
-      <c r="G85" s="1" t="s">
+      <c r="F85" s="6"/>
+      <c r="G85" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="5">
         <v>2</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A86">
+    <row r="86" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
         <v>75</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="5">
         <v>3300</v>
       </c>
-      <c r="G86" s="1" t="s">
+      <c r="F86" s="6"/>
+      <c r="G86" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="5">
         <v>3</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A87">
+    <row r="87" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
         <v>75</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="5">
         <v>4398</v>
       </c>
-      <c r="G87" s="1" t="s">
+      <c r="F87" s="6"/>
+      <c r="G87" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="5">
         <v>2</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87" s="5" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5454,23 +5653,24 @@
         <v>226</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A89">
+    <row r="89" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
         <v>76</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="5">
         <v>-2200</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="F89" s="6"/>
+      <c r="G89" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="5">
         <v>2</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I89" s="5" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5491,83 +5691,93 @@
         <v>234</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A91">
+    <row r="91" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
         <v>76</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="5">
         <v>4000</v>
       </c>
-      <c r="G91" s="1" t="s">
+      <c r="F91" s="6"/>
+      <c r="G91" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="5">
         <v>2</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A92">
+    <row r="92" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
         <v>76</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="5">
         <v>4500</v>
       </c>
-      <c r="G92" s="1" t="s">
+      <c r="F92" s="6"/>
+      <c r="G92" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="5">
         <v>3</v>
       </c>
-      <c r="I92" t="s">
+      <c r="I92" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A93">
+    <row r="93" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
         <v>76</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="5">
         <v>5200</v>
       </c>
-      <c r="G93" s="1" t="s">
+      <c r="F93" s="6"/>
+      <c r="G93" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="5">
         <v>3</v>
       </c>
-      <c r="I93" t="s">
+      <c r="I93" s="5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A94">
+    <row r="94" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="7">
         <v>76</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="7">
         <v>5200</v>
       </c>
-      <c r="G94" s="1" t="s">
+      <c r="D94" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="E94" s="7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="7">
         <v>2</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I94" s="7" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5588,43 +5798,45 @@
         <v>226</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A96">
+    <row r="96" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
         <v>77</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="5">
         <v>-3900</v>
       </c>
-      <c r="G96" s="1" t="s">
+      <c r="F96" s="6"/>
+      <c r="G96" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="5">
         <v>3</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I96" s="5" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A97">
+    <row r="97" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
         <v>77</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="5">
         <v>-3050</v>
       </c>
-      <c r="G97" s="1" t="s">
+      <c r="F97" s="6"/>
+      <c r="G97" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="5">
         <v>2</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" s="5" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5645,83 +5857,87 @@
         <v>234</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A99">
+    <row r="99" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
         <v>77</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="5">
         <v>5500</v>
       </c>
-      <c r="G99" s="1" t="s">
+      <c r="F99" s="6"/>
+      <c r="G99" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="5">
         <v>2</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A100">
+    <row r="100" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
         <v>77</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="5">
         <v>6000</v>
       </c>
-      <c r="G100" s="1" t="s">
+      <c r="F100" s="6"/>
+      <c r="G100" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="5">
         <v>3</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A101">
+    <row r="101" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
         <v>78</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="5">
         <v>-4500</v>
       </c>
-      <c r="G101" s="1" t="s">
+      <c r="F101" s="6"/>
+      <c r="G101" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="5">
         <v>3</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I101" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A102">
+    <row r="102" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
         <v>78</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="5">
         <v>-3700</v>
       </c>
-      <c r="G102" s="1" t="s">
+      <c r="F102" s="6"/>
+      <c r="G102" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="5">
         <v>2</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102" s="5" t="s">
         <v>236</v>
       </c>
     </row>
@@ -5742,23 +5958,24 @@
         <v>243</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A104">
+    <row r="104" spans="1:9" s="5" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
         <v>79</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="5">
         <v>-5200</v>
       </c>
-      <c r="G104" s="1" t="s">
+      <c r="F104" s="6"/>
+      <c r="G104" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="5">
         <v>3</v>
       </c>
-      <c r="I104" t="s">
+      <c r="I104" s="5" t="s">
         <v>242</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new TM ions into half filled shell list
</commit_message>
<xml_diff>
--- a/Documentation/Ion data.xlsx
+++ b/Documentation/Ion data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shannon\Documents\0Schoolwork\PyCrystalField-mod\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EAB19D-8C6A-4A50-B0AB-63A16E267815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7C3F85-E88D-49C1-A42B-005A2A9103DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11730" yWindow="15" windowWidth="11880" windowHeight="12765" xr2:uid="{EFD51521-650C-4408-8F21-64BF005F46EA}"/>
+    <workbookView xWindow="12225" yWindow="30" windowWidth="11880" windowHeight="12765" xr2:uid="{EFD51521-650C-4408-8F21-64BF005F46EA}"/>
   </bookViews>
   <sheets>
     <sheet name="TM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="250">
   <si>
     <t>Cu2+</t>
   </si>
@@ -3166,6 +3166,9 @@
       </rPr>
       <t>2</t>
     </r>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -3258,7 +3261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3268,8 +3271,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3608,8 +3609,8 @@
   <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81:E82"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,6 +3713,9 @@
       <c r="E4">
         <v>0.58699999999999997</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>30</v>
       </c>
@@ -3755,6 +3759,9 @@
       <c r="E6">
         <v>0.79300000000000004</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>157</v>
       </c>
@@ -3781,6 +3788,9 @@
       <c r="E7">
         <v>0.45600000000000002</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
@@ -3807,6 +3817,9 @@
       <c r="E8">
         <v>0.29499999999999998</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>30</v>
       </c>
@@ -3850,6 +3863,9 @@
       <c r="E10">
         <v>0.60499999999999998</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>164</v>
       </c>
@@ -3876,6 +3892,9 @@
       <c r="E11">
         <v>0.36199999999999999</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>157</v>
       </c>
@@ -3886,57 +3905,61 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>24</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12">
         <v>329</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12">
         <v>0.34899999999999998</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12">
         <v>0.24099999999999999</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12">
         <v>3</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>24</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13">
         <v>383</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13">
         <v>0.17399999999999999</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3973,6 +3996,9 @@
       <c r="E15">
         <v>0.47499999999999998</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>165</v>
       </c>
@@ -3999,6 +4025,9 @@
       <c r="E16">
         <v>0.29299999999999998</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>164</v>
       </c>
@@ -4025,6 +4054,9 @@
       <c r="E17">
         <v>0.20100000000000001</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>157</v>
       </c>
@@ -4035,57 +4067,61 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>25</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18">
         <v>479</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18">
         <v>0.27600000000000002</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18">
         <v>0.14599999999999999</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8" t="s">
+      <c r="F18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18">
         <v>3</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>25</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19">
         <v>542</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19">
         <v>0.245</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19">
         <v>0.112</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19">
         <v>2</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4122,6 +4158,9 @@
       <c r="E21">
         <v>0.38</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>164</v>
       </c>
@@ -4148,6 +4187,9 @@
       <c r="E22">
         <v>0.24</v>
       </c>
+      <c r="F22" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>165</v>
       </c>
@@ -4174,6 +4216,9 @@
       <c r="E23">
         <v>0.31</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>157</v>
       </c>
@@ -4200,6 +4245,9 @@
       <c r="E24">
         <v>0.2</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>164</v>
       </c>
@@ -4249,6 +4297,9 @@
       <c r="E26">
         <v>0.25600000000000001</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G26" s="1" t="s">
         <v>164</v>
       </c>
@@ -4275,6 +4326,9 @@
       <c r="E27">
         <v>0.16800000000000001</v>
       </c>
+      <c r="F27" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G27" s="1" t="s">
         <v>157</v>
       </c>
@@ -4318,6 +4372,9 @@
       <c r="E29">
         <v>0.21</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>30</v>
       </c>
@@ -4379,30 +4436,32 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>39</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" t="s">
         <v>160</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33">
         <v>290</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33">
         <v>1.577</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33">
         <v>4.4080000000000004</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8" t="s">
+      <c r="F33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33">
         <v>2</v>
       </c>
-      <c r="I33" s="7" t="s">
+      <c r="I33" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4444,716 +4503,748 @@
         <v>203</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+    <row r="36" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>40</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" t="s">
         <v>162</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36">
         <v>428</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36">
         <v>1.3129999999999999</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36">
         <v>3.09</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8" t="s">
+      <c r="F36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36">
         <v>3</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I36" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>40</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" t="s">
         <v>163</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37">
         <v>500</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37">
         <v>2.645</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37">
         <v>2.0129999999999999</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8" t="s">
+      <c r="F37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37">
         <v>2</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="I37" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+    <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>40</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38" s="7" t="s">
+      <c r="I38" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+    <row r="39" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>41</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39">
         <v>677</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39">
         <v>0.96</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39">
         <v>1.573</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8" t="s">
+      <c r="F39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39">
         <v>3</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I39" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
+    <row r="40" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>41</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" t="s">
         <v>52</v>
       </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8" t="s">
+      <c r="G40" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="I40" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
+    <row r="41" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>42</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41">
         <v>714</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41">
         <v>0.96899999999999997</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41">
         <v>1.7050000000000001</v>
       </c>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8" t="s">
+      <c r="F41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41">
         <v>2</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I41" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+    <row r="42" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>42</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42">
         <v>836</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42">
         <v>0.83899999999999997</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42">
         <v>1.2050000000000001</v>
       </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8" t="s">
+      <c r="F42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42">
         <v>3</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I42" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+    <row r="43" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43">
         <v>972</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43">
         <v>0.747</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43">
         <v>0.91600000000000004</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H43" s="7">
+      <c r="H43">
         <v>3</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I43" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44">
         <v>1031</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44">
         <v>0.67600000000000005</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44">
         <v>0.72799999999999998</v>
       </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8" t="s">
+      <c r="F44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H44">
         <v>2</v>
       </c>
-      <c r="I44" s="7" t="s">
+      <c r="I44" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+    <row r="45" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>42</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" t="s">
         <v>56</v>
       </c>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8" t="s">
+      <c r="G45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45">
         <v>0</v>
       </c>
-      <c r="I45" s="7" t="s">
+      <c r="I45" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
+    <row r="46" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>43</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46">
         <v>1150</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46">
         <v>0.67400000000000004</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46">
         <v>0.752</v>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8" t="s">
+      <c r="F46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46">
         <v>3</v>
       </c>
-      <c r="I46" s="7" t="s">
+      <c r="I46" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
+    <row r="47" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>43</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" t="s">
         <v>57</v>
       </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H47" s="7">
+      <c r="H47">
         <v>0</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I47" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+    <row r="48" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>44</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48">
         <v>-942</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48">
         <v>0.75700000000000001</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48">
         <v>1.052</v>
       </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8" t="s">
+      <c r="F48" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48">
         <v>2</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I48" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+    <row r="49" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>44</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49">
         <v>1177</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49">
         <v>0.67400000000000004</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49">
         <v>0.79</v>
       </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8" t="s">
+      <c r="F49" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49">
         <v>0</v>
       </c>
-      <c r="I49" s="7" t="s">
+      <c r="I49" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+    <row r="50" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>44</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" t="s">
         <v>59</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50">
         <v>1350</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50">
         <v>0.60699999999999998</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50">
         <v>0.61299999999999999</v>
       </c>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8" t="s">
+      <c r="F50" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50">
         <v>2</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I50" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+    <row r="51" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>44</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51">
         <v>1700</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51">
         <v>0.51500000000000001</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51">
         <v>0.42</v>
       </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8" t="s">
+      <c r="F51" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H51" s="7">
+      <c r="H51">
         <v>3</v>
       </c>
-      <c r="I51" s="7" t="s">
+      <c r="I51" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+    <row r="52" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>44</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" t="s">
         <v>61</v>
       </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H52" s="7">
+      <c r="H52">
         <v>0</v>
       </c>
-      <c r="I52" s="7" t="s">
+      <c r="I52" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+    <row r="53" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>45</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53">
         <v>-1194</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53">
         <v>0.68</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53">
         <v>0.85</v>
       </c>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8" t="s">
+      <c r="F53" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H53">
         <v>3</v>
       </c>
-      <c r="I53" s="7" t="s">
+      <c r="I53" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+    <row r="54" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>45</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" t="s">
         <v>18</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54">
         <v>-1360</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54">
         <v>0.61</v>
       </c>
-      <c r="E54" s="7">
+      <c r="E54">
         <v>0.64900000000000002</v>
       </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8" t="s">
+      <c r="F54" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H54" s="7">
+      <c r="H54">
         <v>2</v>
       </c>
-      <c r="I54" s="7" t="s">
+      <c r="I54" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
+    <row r="55" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>45</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55">
         <v>1350</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55">
         <v>0.55300000000000005</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55">
         <v>0.51200000000000001</v>
       </c>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8" t="s">
+      <c r="F55" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="H55" s="7">
+      <c r="H55">
         <v>0</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I55" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
+    <row r="56" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>46</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56">
         <v>-1293</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56">
         <v>0.61699999999999999</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56">
         <v>0.70499999999999996</v>
       </c>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8" t="s">
+      <c r="F56" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H56" s="7">
+      <c r="H56">
         <v>3</v>
       </c>
-      <c r="I56" s="7" t="s">
+      <c r="I56" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
+    <row r="57" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>46</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57">
         <v>-1211</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57">
         <v>0.55500000000000005</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57">
         <v>0.54</v>
       </c>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8" t="s">
+      <c r="F57" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57">
         <v>3</v>
       </c>
-      <c r="I57" s="7" t="s">
+      <c r="I57" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
+    <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>46</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58">
         <v>-1830</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58">
         <v>0.55300000000000005</v>
       </c>
-      <c r="E58" s="7">
+      <c r="E58">
         <v>0.53500000000000003</v>
       </c>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8" t="s">
+      <c r="F58" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H58">
         <v>2</v>
       </c>
-      <c r="I58" s="7" t="s">
+      <c r="I58" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
+    <row r="59" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>47</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" t="s">
         <v>65</v>
       </c>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8" t="s">
+      <c r="G59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59">
         <v>0</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I59" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
+    <row r="60" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>47</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" t="s">
         <v>166</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60">
         <v>-1843</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60">
         <v>0.55900000000000005</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60">
         <v>0.57899999999999996</v>
       </c>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8" t="s">
+      <c r="F60" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H60">
         <v>2</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I60" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="7">
+    <row r="61" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>47</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" t="s">
         <v>167</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61">
         <v>-1930</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D61">
         <v>0.50700000000000001</v>
       </c>
-      <c r="E61" s="7">
+      <c r="E61">
         <v>0.45</v>
       </c>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8" t="s">
+      <c r="F61" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H61" s="7">
+      <c r="H61">
         <v>3</v>
       </c>
-      <c r="I61" s="7" t="s">
+      <c r="I61" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
+    <row r="62" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>48</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" t="s">
         <v>168</v>
       </c>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8" t="s">
+      <c r="G62" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H62" s="7">
+      <c r="H62">
         <v>0</v>
       </c>
-      <c r="I62" s="7" t="s">
+      <c r="I62" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="7">
+    <row r="63" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>48</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" t="s">
         <v>66</v>
       </c>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8" t="s">
+      <c r="G63" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H63" s="7">
+      <c r="H63">
         <v>0</v>
       </c>
-      <c r="I63" s="7" t="s">
+      <c r="I63" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="7">
+    <row r="64" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>48</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" t="s">
         <v>223</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64">
         <v>-2325</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64">
         <v>0.46600000000000003</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64">
         <v>0.38300000000000001</v>
       </c>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8" t="s">
+      <c r="F64" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H64" s="7">
+      <c r="H64">
         <v>2</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I64" t="s">
         <v>218</v>
       </c>
     </row>
@@ -5259,57 +5350,61 @@
         <v>217</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="7">
+    <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>72</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" t="s">
         <v>172</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71">
         <v>1370</v>
       </c>
-      <c r="D71" s="7">
+      <c r="D71">
         <v>0.159</v>
       </c>
-      <c r="E71" s="7">
+      <c r="E71">
         <v>6.3E-2</v>
       </c>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8" t="s">
+      <c r="F71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H71" s="7">
+      <c r="H71">
         <v>3</v>
       </c>
-      <c r="I71" s="7" t="s">
+      <c r="I71" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="72" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="7">
+    <row r="72" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>72</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" t="s">
         <v>173</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72">
         <v>1877</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D72">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72">
         <v>0.01</v>
       </c>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8" t="s">
+      <c r="F72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H72" s="7">
+      <c r="H72">
         <v>2</v>
       </c>
-      <c r="I72" s="7" t="s">
+      <c r="I72" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5357,7 +5452,9 @@
       <c r="C75" s="5">
         <v>2000</v>
       </c>
-      <c r="F75" s="6"/>
+      <c r="F75" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G75" s="6" t="s">
         <v>157</v>
       </c>
@@ -5378,7 +5475,9 @@
       <c r="C76" s="5">
         <v>2254</v>
       </c>
-      <c r="F76" s="6"/>
+      <c r="F76" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G76" s="6" t="s">
         <v>31</v>
       </c>
@@ -5399,7 +5498,9 @@
       <c r="C77" s="5">
         <v>2643</v>
       </c>
-      <c r="F77" s="6"/>
+      <c r="F77" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G77" s="6" t="s">
         <v>30</v>
       </c>
@@ -5437,7 +5538,9 @@
       <c r="C79" s="5">
         <v>2500</v>
       </c>
-      <c r="F79" s="6"/>
+      <c r="F79" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G79" s="6" t="s">
         <v>164</v>
       </c>
@@ -5458,7 +5561,9 @@
       <c r="C80" s="5">
         <v>2686</v>
       </c>
-      <c r="F80" s="6"/>
+      <c r="F80" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G80" s="6" t="s">
         <v>157</v>
       </c>
@@ -5479,10 +5584,10 @@
       <c r="C81">
         <v>3108</v>
       </c>
-      <c r="D81" s="9">
+      <c r="D81" s="7">
         <v>0.125</v>
       </c>
-      <c r="E81" s="9">
+      <c r="E81" s="7">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F81" s="1" t="s">
@@ -5508,10 +5613,10 @@
       <c r="C82">
         <v>3483</v>
       </c>
-      <c r="D82" s="9">
+      <c r="D82" s="7">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E82" s="9">
+      <c r="E82" s="7">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F82" s="1" t="s">
@@ -5583,7 +5688,9 @@
       <c r="C85" s="5">
         <v>5800</v>
       </c>
-      <c r="F85" s="6"/>
+      <c r="F85" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G85" s="6" t="s">
         <v>164</v>
       </c>
@@ -5604,7 +5711,9 @@
       <c r="C86" s="5">
         <v>3300</v>
       </c>
-      <c r="F86" s="6"/>
+      <c r="F86" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G86" s="6" t="s">
         <v>157</v>
       </c>
@@ -5625,7 +5734,9 @@
       <c r="C87" s="5">
         <v>4398</v>
       </c>
-      <c r="F87" s="6"/>
+      <c r="F87" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G87" s="6" t="s">
         <v>30</v>
       </c>
@@ -5663,7 +5774,9 @@
       <c r="C89" s="5">
         <v>-2200</v>
       </c>
-      <c r="F89" s="6"/>
+      <c r="F89" s="6" t="s">
+        <v>249</v>
+      </c>
       <c r="G89" s="6" t="s">
         <v>164</v>
       </c>
@@ -5701,7 +5814,9 @@
       <c r="C91" s="5">
         <v>4000</v>
       </c>
-      <c r="F91" s="6"/>
+      <c r="F91" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G91" s="6" t="s">
         <v>164</v>
       </c>
@@ -5722,7 +5837,9 @@
       <c r="C92" s="5">
         <v>4500</v>
       </c>
-      <c r="F92" s="6"/>
+      <c r="F92" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G92" s="6" t="s">
         <v>157</v>
       </c>
@@ -5743,7 +5860,9 @@
       <c r="C93" s="5">
         <v>5200</v>
       </c>
-      <c r="F93" s="6"/>
+      <c r="F93" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G93" s="6" t="s">
         <v>31</v>
       </c>
@@ -5754,30 +5873,32 @@
         <v>233</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="7">
+    <row r="94" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94">
         <v>76</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B94" t="s">
         <v>239</v>
       </c>
-      <c r="C94" s="7">
+      <c r="C94">
         <v>5200</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D94">
         <v>0.06</v>
       </c>
-      <c r="E94" s="7">
+      <c r="E94">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8" t="s">
+      <c r="F94" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G94" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H94" s="7">
+      <c r="H94">
         <v>2</v>
       </c>
-      <c r="I94" s="7" t="s">
+      <c r="I94" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5808,7 +5929,9 @@
       <c r="C96" s="5">
         <v>-3900</v>
       </c>
-      <c r="F96" s="6"/>
+      <c r="F96" s="6" t="s">
+        <v>249</v>
+      </c>
       <c r="G96" s="6" t="s">
         <v>157</v>
       </c>
@@ -5829,7 +5952,9 @@
       <c r="C97" s="5">
         <v>-3050</v>
       </c>
-      <c r="F97" s="6"/>
+      <c r="F97" s="6" t="s">
+        <v>249</v>
+      </c>
       <c r="G97" s="6" t="s">
         <v>164</v>
       </c>
@@ -5867,7 +5992,9 @@
       <c r="C99" s="5">
         <v>5500</v>
       </c>
-      <c r="F99" s="6"/>
+      <c r="F99" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G99" s="6" t="s">
         <v>164</v>
       </c>
@@ -5888,7 +6015,9 @@
       <c r="C100" s="5">
         <v>6000</v>
       </c>
-      <c r="F100" s="6"/>
+      <c r="F100" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G100" s="6" t="s">
         <v>157</v>
       </c>
@@ -5909,7 +6038,9 @@
       <c r="C101" s="5">
         <v>-4500</v>
       </c>
-      <c r="F101" s="6"/>
+      <c r="F101" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G101" s="6" t="s">
         <v>31</v>
       </c>
@@ -5930,7 +6061,9 @@
       <c r="C102" s="5">
         <v>-3700</v>
       </c>
-      <c r="F102" s="6"/>
+      <c r="F102" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G102" s="6" t="s">
         <v>164</v>
       </c>
@@ -5968,7 +6101,9 @@
       <c r="C104" s="5">
         <v>-5200</v>
       </c>
-      <c r="F104" s="6"/>
+      <c r="F104" s="6" t="s">
+        <v>249</v>
+      </c>
       <c r="G104" s="6" t="s">
         <v>31</v>
       </c>

</xml_diff>